<commit_message>
cahier de test mis à jour
</commit_message>
<xml_diff>
--- a/annexes/Cahier_de_test_Rosetta_GrpA.xlsx
+++ b/annexes/Cahier_de_test_Rosetta_GrpA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Travail\Projet\rosetta\annexes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB969BA-8D3E-D143-8C66-4CBC45ED09B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D63C2DA-13F5-4F6B-9CB1-4BCF97E40AEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="2" r:id="rId1"/>
@@ -1696,7 +1696,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1994,34 +1994,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D569B6-B3CB-4EA1-907F-9E75FD9F6494}">
   <dimension ref="A1:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G112" sqref="G112"/>
+    <sheetView tabSelected="1" topLeftCell="B74" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.16796875" customWidth="1"/>
-    <col min="2" max="2" width="19.234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.58203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="120.80078125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="85.421875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.41015625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.265625" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="120.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="85.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="49" t="s">
         <v>138</v>
       </c>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="26" t="s">
         <v>267</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="26" t="s">
         <v>15</v>
       </c>
@@ -2048,7 +2048,7 @@
       <c r="F5" s="41"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
         <v>139</v>
       </c>
@@ -2066,7 +2066,7 @@
       </c>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="30" t="s">
         <v>140</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="27" t="s">
         <v>145</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="28" t="s">
         <v>146</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="30" t="s">
         <v>152</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="27" t="s">
         <v>155</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="30" t="s">
         <v>158</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="27" t="s">
         <v>208</v>
@@ -2186,7 +2186,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="27" t="s">
         <v>209</v>
@@ -2204,7 +2204,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="27" t="s">
         <v>210</v>
@@ -2222,7 +2222,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="27" t="s">
         <v>211</v>
@@ -2240,7 +2240,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="26" t="s">
         <v>19</v>
@@ -2250,7 +2250,7 @@
       <c r="E17" s="25"/>
       <c r="F17" s="26"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="27" t="s">
         <v>167</v>
@@ -2268,7 +2268,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="30" t="s">
         <v>170</v>
@@ -2286,7 +2286,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="27" t="s">
         <v>173</v>
@@ -2304,7 +2304,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="28" t="s">
         <v>177</v>
@@ -2322,7 +2322,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="27" t="s">
         <v>178</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="28" t="s">
         <v>179</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="27" t="s">
         <v>204</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="15" t="s">
         <v>205</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="27" t="s">
         <v>187</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="30" t="s">
         <v>188</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="15" t="s">
         <v>206</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="27" t="s">
         <v>193</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="30" t="s">
         <v>196</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="27" t="s">
         <v>195</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="30" t="s">
         <v>201</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="15" t="s">
         <v>207</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="15" t="s">
         <v>214</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="15" t="s">
         <v>217</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="15" t="s">
         <v>219</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="27" t="s">
         <v>223</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="30" t="s">
         <v>224</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="15" t="s">
         <v>226</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="14" t="s">
         <v>21</v>
       </c>
@@ -2642,7 +2642,7 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="15" t="s">
         <v>233</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="15" t="s">
         <v>235</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="15" t="s">
         <v>238</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="15" t="s">
         <v>239</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" s="27" t="s">
         <v>243</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" s="30" t="s">
         <v>244</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="15" t="s">
         <v>247</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="15" t="s">
         <v>250</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="15" t="s">
         <v>252</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="27" t="s">
         <v>256</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="30" t="s">
         <v>260</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="27" t="s">
         <v>261</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="30" t="s">
         <v>262</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="15" t="s">
         <v>263</v>
       </c>
@@ -2880,18 +2880,18 @@
         <v>368</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F55" s="43"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F56" s="43"/>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="26" t="s">
         <v>267</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="34" t="s">
         <v>272</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="34" t="s">
         <v>273</v>
       </c>
@@ -2942,7 +2942,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="26" t="s">
         <v>43</v>
       </c>
@@ -2951,7 +2951,7 @@
       <c r="E61" s="26"/>
       <c r="F61" s="26"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="15" t="s">
         <v>276</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63" s="15" t="s">
         <v>279</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="15" t="s">
         <v>284</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="26" t="s">
         <v>15</v>
       </c>
@@ -3011,7 +3011,7 @@
       <c r="E65" s="26"/>
       <c r="F65" s="26"/>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" s="27" t="s">
         <v>293</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" s="30" t="s">
         <v>294</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="27" t="s">
         <v>295</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" s="28" t="s">
         <v>296</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" s="28" t="s">
         <v>297</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="27" t="s">
         <v>288</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" s="28" t="s">
         <v>289</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" s="28" t="s">
         <v>291</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" s="27" t="s">
         <v>299</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" s="27" t="s">
         <v>300</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" s="27" t="s">
         <v>301</v>
       </c>
@@ -3199,7 +3199,7 @@
       </c>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="27" t="s">
         <v>302</v>
       </c>
@@ -3217,7 +3217,7 @@
       </c>
       <c r="H77" s="43"/>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" s="26" t="s">
         <v>19</v>
       </c>
@@ -3226,7 +3226,7 @@
       <c r="E78" s="25"/>
       <c r="F78" s="26"/>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="27" t="s">
         <v>332</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" s="27" t="s">
         <v>333</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81" s="27" t="s">
         <v>334</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" s="27" t="s">
         <v>335</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" s="27" t="s">
         <v>336</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" s="27" t="s">
         <v>337</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" s="27" t="s">
         <v>338</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" s="15" t="s">
         <v>339</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" s="27" t="s">
         <v>340</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" s="27" t="s">
         <v>341</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" s="15" t="s">
         <v>342</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" s="27" t="s">
         <v>343</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91" s="27" t="s">
         <v>344</v>
       </c>
@@ -3450,7 +3450,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B92" s="27" t="s">
         <v>345</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B93" s="27" t="s">
         <v>346</v>
       </c>
@@ -3484,7 +3484,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94" s="15" t="s">
         <v>347</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95" s="15" t="s">
         <v>348</v>
       </c>
@@ -3518,7 +3518,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96" s="15" t="s">
         <v>349</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B97" s="15" t="s">
         <v>350</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B98" s="27" t="s">
         <v>351</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B99" s="30" t="s">
         <v>352</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B100" s="15" t="s">
         <v>353</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B101" s="14" t="s">
         <v>21</v>
       </c>
@@ -3612,7 +3612,7 @@
       <c r="E101" s="51"/>
       <c r="F101" s="52"/>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B102" s="15" t="s">
         <v>354</v>
       </c>
@@ -3625,11 +3625,11 @@
       <c r="E102" s="32" t="s">
         <v>232</v>
       </c>
-      <c r="F102" s="48" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F102" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B103" s="15" t="s">
         <v>355</v>
       </c>
@@ -3642,11 +3642,11 @@
       <c r="E103" s="32" t="s">
         <v>236</v>
       </c>
-      <c r="F103" s="48" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F103" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B104" s="15" t="s">
         <v>356</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B105" s="15" t="s">
         <v>357</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B106" s="27" t="s">
         <v>358</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B107" s="30" t="s">
         <v>359</v>
       </c>
@@ -3714,7 +3714,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B108" s="15" t="s">
         <v>360</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B109" s="15" t="s">
         <v>361</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B110" s="15" t="s">
         <v>362</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B111" s="27" t="s">
         <v>363</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B112" s="27" t="s">
         <v>364</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B113" s="27" t="s">
         <v>365</v>
       </c>
@@ -3816,7 +3816,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B114" s="27" t="s">
         <v>366</v>
       </c>
@@ -3833,7 +3833,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B115" s="15" t="s">
         <v>367</v>
       </c>
@@ -3850,12 +3850,12 @@
         <v>304</v>
       </c>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B117" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B118" s="26" t="s">
         <v>267</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B119" s="27" t="s">
         <v>305</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B120" s="28" t="s">
         <v>306</v>
       </c>
@@ -3906,7 +3906,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B121" s="30" t="s">
         <v>310</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B122" s="15" t="s">
         <v>313</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B123" s="27" t="s">
         <v>318</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B124" s="28" t="s">
         <v>319</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B125" s="30" t="s">
         <v>320</v>
       </c>
@@ -3991,7 +3991,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B126" s="27" t="s">
         <v>323</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B127" s="30" t="s">
         <v>325</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B128" s="15" t="s">
         <v>329</v>
       </c>
@@ -4062,30 +4062,30 @@
       <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="127.125" customWidth="1"/>
-    <col min="4" max="4" width="18.0234375" customWidth="1"/>
-    <col min="5" max="5" width="26.09765625" customWidth="1"/>
-    <col min="7" max="7" width="11.43359375" customWidth="1"/>
-    <col min="9" max="9" width="16.27734375" customWidth="1"/>
-    <col min="10" max="10" width="43.58203125" customWidth="1"/>
+    <col min="3" max="3" width="127.140625" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="43.5703125" customWidth="1"/>
     <col min="11" max="11" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="56" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="56"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -4104,7 +4104,7 @@
       <c r="G4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>15</v>
       </c>
@@ -4115,7 +4115,7 @@
       <c r="G5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="15" t="s">
         <v>23</v>
@@ -4137,7 +4137,7 @@
       <c r="J6" s="21"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="15" t="s">
         <v>24</v>
@@ -4159,7 +4159,7 @@
       <c r="J7" s="21"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>25</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>26</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>58</v>
       </c>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="G10" s="13"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
         <v>59</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
         <v>60</v>
       </c>
@@ -4245,7 +4245,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>19</v>
       </c>
@@ -4259,7 +4259,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="15" t="s">
         <v>27</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
         <v>28</v>
       </c>
@@ -4293,7 +4293,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
         <v>29</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="15" t="s">
         <v>30</v>
       </c>
@@ -4327,7 +4327,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="15" t="s">
         <v>31</v>
       </c>
@@ -4345,7 +4345,7 @@
       </c>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
         <v>32</v>
       </c>
@@ -4363,7 +4363,7 @@
       </c>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="15" t="s">
         <v>74</v>
       </c>
@@ -4381,7 +4381,7 @@
       </c>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="15" t="s">
         <v>75</v>
       </c>
@@ -4399,7 +4399,7 @@
       </c>
       <c r="G21" s="13"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="15" t="s">
         <v>76</v>
       </c>
@@ -4417,7 +4417,7 @@
       </c>
       <c r="G22" s="13"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="15" t="s">
         <v>77</v>
       </c>
@@ -4435,7 +4435,7 @@
       </c>
       <c r="G23" s="13"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="15" t="s">
         <v>78</v>
       </c>
@@ -4453,7 +4453,7 @@
       </c>
       <c r="G24" s="13"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="15" t="s">
         <v>79</v>
       </c>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="G25" s="13"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="15" t="s">
         <v>80</v>
       </c>
@@ -4489,7 +4489,7 @@
       </c>
       <c r="G26" s="13"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="15" t="s">
         <v>81</v>
       </c>
@@ -4507,7 +4507,7 @@
       </c>
       <c r="G27" s="13"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="15" t="s">
         <v>82</v>
       </c>
@@ -4525,7 +4525,7 @@
       </c>
       <c r="G28" s="13"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
         <v>21</v>
       </c>
@@ -4539,7 +4539,7 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="15" t="s">
         <v>33</v>
       </c>
@@ -4557,7 +4557,7 @@
       </c>
       <c r="G30" s="13"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="15" t="s">
         <v>34</v>
       </c>
@@ -4575,7 +4575,7 @@
       </c>
       <c r="G31" s="13"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="15" t="s">
         <v>35</v>
       </c>
@@ -4593,7 +4593,7 @@
       </c>
       <c r="G32" s="13"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B33" s="15" t="s">
         <v>37</v>
       </c>
@@ -4611,7 +4611,7 @@
       </c>
       <c r="G33" s="13"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B34" s="15" t="s">
         <v>38</v>
       </c>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="G34" s="13"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B35" s="15" t="s">
         <v>94</v>
       </c>
@@ -4647,7 +4647,7 @@
       </c>
       <c r="G35" s="13"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36" s="15" t="s">
         <v>95</v>
       </c>
@@ -4665,7 +4665,7 @@
       </c>
       <c r="G36" s="13"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B37" s="15" t="s">
         <v>96</v>
       </c>
@@ -4683,7 +4683,7 @@
       </c>
       <c r="G37" s="13"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B38" s="15" t="s">
         <v>97</v>
       </c>
@@ -4701,7 +4701,7 @@
       </c>
       <c r="G38" s="13"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" s="15" t="s">
         <v>98</v>
       </c>
@@ -4719,7 +4719,7 @@
       </c>
       <c r="G39" s="13"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40" s="15" t="s">
         <v>99</v>
       </c>
@@ -4737,19 +4737,19 @@
       </c>
       <c r="G40" s="13"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
         <v>0</v>
       </c>
@@ -4773,7 +4773,7 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="15" t="s">
         <v>41</v>
@@ -4796,7 +4796,7 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45" s="14" t="s">
         <v>43</v>
       </c>
@@ -4810,7 +4810,7 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B46" s="15" t="s">
         <v>44</v>
       </c>
@@ -4827,7 +4827,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B47" s="15" t="s">
         <v>45</v>
       </c>
@@ -4845,7 +4845,7 @@
       </c>
       <c r="G47" s="13"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B48" s="15" t="s">
         <v>46</v>
       </c>
@@ -4863,7 +4863,7 @@
       </c>
       <c r="G48" s="13"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B49" s="14" t="s">
         <v>15</v>
       </c>
@@ -4874,7 +4874,7 @@
       <c r="G49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="15" t="s">
         <v>103</v>
@@ -4896,7 +4896,7 @@
       <c r="J50" s="21"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="15" t="s">
         <v>104</v>
@@ -4918,7 +4918,7 @@
       <c r="J51" s="21"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="15" t="s">
         <v>105</v>
       </c>
@@ -4935,7 +4935,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="15" t="s">
         <v>106</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="15" t="s">
         <v>107</v>
       </c>
@@ -4970,7 +4970,7 @@
       </c>
       <c r="G54" s="13"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B55" s="15" t="s">
         <v>108</v>
       </c>
@@ -4987,7 +4987,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B56" s="15" t="s">
         <v>109</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B57" s="14" t="s">
         <v>19</v>
       </c>
@@ -5018,7 +5018,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B58" s="15" t="s">
         <v>110</v>
       </c>
@@ -5035,7 +5035,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B59" s="15" t="s">
         <v>111</v>
       </c>
@@ -5052,7 +5052,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B60" s="15" t="s">
         <v>112</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B61" s="15" t="s">
         <v>113</v>
       </c>
@@ -5086,7 +5086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B62" s="15" t="s">
         <v>114</v>
       </c>
@@ -5104,7 +5104,7 @@
       </c>
       <c r="G62" s="13"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B63" s="15" t="s">
         <v>115</v>
       </c>
@@ -5122,7 +5122,7 @@
       </c>
       <c r="G63" s="13"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B64" s="15" t="s">
         <v>116</v>
       </c>
@@ -5140,7 +5140,7 @@
       </c>
       <c r="G64" s="13"/>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B65" s="15" t="s">
         <v>117</v>
       </c>
@@ -5158,7 +5158,7 @@
       </c>
       <c r="G65" s="13"/>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B66" s="15" t="s">
         <v>118</v>
       </c>
@@ -5176,7 +5176,7 @@
       </c>
       <c r="G66" s="13"/>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B67" s="15" t="s">
         <v>119</v>
       </c>
@@ -5194,7 +5194,7 @@
       </c>
       <c r="G67" s="13"/>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B68" s="15" t="s">
         <v>120</v>
       </c>
@@ -5212,7 +5212,7 @@
       </c>
       <c r="G68" s="13"/>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69" s="15" t="s">
         <v>121</v>
       </c>
@@ -5230,7 +5230,7 @@
       </c>
       <c r="G69" s="13"/>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B70" s="15" t="s">
         <v>122</v>
       </c>
@@ -5248,7 +5248,7 @@
       </c>
       <c r="G70" s="13"/>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B71" s="15" t="s">
         <v>123</v>
       </c>
@@ -5266,7 +5266,7 @@
       </c>
       <c r="G71" s="13"/>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B72" s="15" t="s">
         <v>124</v>
       </c>
@@ -5284,7 +5284,7 @@
       </c>
       <c r="G72" s="13"/>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B73" s="14" t="s">
         <v>21</v>
       </c>
@@ -5298,7 +5298,7 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B74" s="15" t="s">
         <v>125</v>
       </c>
@@ -5316,7 +5316,7 @@
       </c>
       <c r="G74" s="13"/>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B75" s="15" t="s">
         <v>126</v>
       </c>
@@ -5334,7 +5334,7 @@
       </c>
       <c r="G75" s="13"/>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B76" s="15" t="s">
         <v>127</v>
       </c>
@@ -5352,7 +5352,7 @@
       </c>
       <c r="G76" s="13"/>
     </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B77" s="15" t="s">
         <v>128</v>
       </c>
@@ -5370,7 +5370,7 @@
       </c>
       <c r="G77" s="13"/>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B78" s="15" t="s">
         <v>129</v>
       </c>
@@ -5388,7 +5388,7 @@
       </c>
       <c r="G78" s="13"/>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B79" s="15" t="s">
         <v>130</v>
       </c>
@@ -5406,7 +5406,7 @@
       </c>
       <c r="G79" s="13"/>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B80" s="15" t="s">
         <v>131</v>
       </c>
@@ -5424,7 +5424,7 @@
       </c>
       <c r="G80" s="18"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B81" s="15" t="s">
         <v>132</v>
       </c>
@@ -5442,7 +5442,7 @@
       </c>
       <c r="G81" s="18"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B82" s="15" t="s">
         <v>133</v>
       </c>
@@ -5460,7 +5460,7 @@
       </c>
       <c r="G82" s="18"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B83" s="15" t="s">
         <v>134</v>
       </c>
@@ -5478,7 +5478,7 @@
       </c>
       <c r="G83" s="18"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B84" s="15" t="s">
         <v>135</v>
       </c>
@@ -5496,19 +5496,19 @@
       </c>
       <c r="G84" s="18"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B86" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
         <v>0</v>
       </c>
@@ -5532,7 +5532,7 @@
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="15" t="s">
         <v>51</v>
@@ -5555,7 +5555,7 @@
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="15" t="s">
         <v>52</v>
@@ -5578,7 +5578,7 @@
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="15" t="s">
         <v>100</v>
@@ -5601,7 +5601,7 @@
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="15" t="s">
         <v>101</v>
@@ -5624,7 +5624,7 @@
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
     </row>
-    <row r="92" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="15" t="s">
         <v>102</v>
       </c>
@@ -5642,26 +5642,26 @@
       </c>
       <c r="G92" s="22"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="13"/>
       <c r="E93" s="13"/>
       <c r="F93" s="2"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B95" s="24" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B96" s="55" t="s">
         <v>137</v>
       </c>
       <c r="C96" s="55"/>
       <c r="D96" s="55"/>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="21" t="s">
         <v>136</v>
       </c>

</xml_diff>